<commit_message>
copy style of a cell
</commit_message>
<xml_diff>
--- a/project/File_Copy.xlsx
+++ b/project/File_Copy.xlsx
@@ -1,20 +1,44 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Score" sheetId="2" r:id="rId1"/>
+    <sheet name="Score" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="12">
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>VM1</t>
+  </si>
+  <si>
+    <t>VC1</t>
+  </si>
+  <si>
+    <t>VC2</t>
+  </si>
+  <si>
+    <t>VC3</t>
+  </si>
+  <si>
+    <t>VC4</t>
+  </si>
+  <si>
+    <t>VC5</t>
+  </si>
+  <si>
+    <t>VC6</t>
+  </si>
   <si>
     <t>G</t>
   </si>
@@ -26,65 +50,48 @@
   </si>
   <si>
     <t>NA</t>
-  </si>
-  <si>
-    <t>ID</t>
-  </si>
-  <si>
-    <t>VM1</t>
-  </si>
-  <si>
-    <t>VC1</t>
-  </si>
-  <si>
-    <t>VC2</t>
-  </si>
-  <si>
-    <t>VC3</t>
-  </si>
-  <si>
-    <t>VC4</t>
-  </si>
-  <si>
-    <t>VC5</t>
-  </si>
-  <si>
-    <t>VC6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="4">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <i/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <b val="1"/>
+      <color theme="1"/>
       <sz val="11"/>
+    </font>
+    <font>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+      <b val="1"/>
+      <i val="1"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <sz val="11"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -92,6 +99,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -121,30 +134,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="7">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf borderId="1" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="3" fontId="2" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf borderId="1" fillId="2" fontId="3" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -434,225 +442,229 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:H8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J11" sqref="J11"/>
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="F1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" s="3">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2" t="s">
+      <c r="H2" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row customHeight="1" ht="23.25" r="3" spans="1:8">
+      <c r="A3" s="2" t="n">
         <v>2</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G2" s="2" t="s">
+      <c r="B3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" s="3">
-        <v>2</v>
-      </c>
-      <c r="B3" s="5" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" s="3">
-        <v>3</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="3">
+      <c r="B4" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="2" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>2</v>
+      <c r="B5" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>10</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="3">
+        <v>8</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="2" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="3">
+      <c r="B6" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" s="2" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="3">
+      <c r="B7" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8">
+      <c r="A8" s="2" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="C8" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>0</v>
+      <c r="B8" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>